<commit_message>
changement du nom de la planif
</commit_message>
<xml_diff>
--- a/PNF-V2.xlsx
+++ b/PNF-V2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26019"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hessoit.sharepoint.com/sites/GREP896/Documents partages/General/Livrable/Livrable A3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thoma\Downloads\Bachelor Marc\gampy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="654" documentId="8_{753257B4-B46C-4DCC-AF09-40496BF9DDB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{42BFD046-07FB-4E3E-9636-BE520A2CE95D}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6608DBB-A87C-4B5A-AF51-1849521DE698}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39210" yWindow="60" windowWidth="37710" windowHeight="21840" xr2:uid="{6ACCAD28-7B53-4994-B276-760184E4CB6E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{6ACCAD28-7B53-4994-B276-760184E4CB6E}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="65">
   <si>
-    <t>Sparkling Event</t>
-  </si>
-  <si>
     <t>HEG Genève</t>
   </si>
   <si>
@@ -234,6 +231,9 @@
   </si>
   <si>
     <t xml:space="preserve"> . . . [ Level 4 Task ]</t>
+  </si>
+  <si>
+    <t>GAMPY</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
     <numFmt numFmtId="165" formatCode="ddd\ dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="m/d/yyyy\ \(dddd\)"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -957,7 +957,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="fr-FR"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -2769,7 +2769,7 @@
                     <a:cs typeface="+mn-cs"/>
                   </a:defRPr>
                 </a:pPr>
-                <a:endParaRPr lang="en-US"/>
+                <a:endParaRPr lang="fr-FR"/>
               </a:p>
             </c:txPr>
             <c:dLblPos val="ctr"/>
@@ -3305,7 +3305,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="451296576"/>
@@ -3368,7 +3368,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="fr-FR"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="451276608"/>
@@ -3410,7 +3410,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="fr-FR"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -4008,7 +4008,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -4307,25 +4307,25 @@
   <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.85546875" customWidth="1"/>
-    <col min="2" max="2" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5703125" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
-    <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.81640625" customWidth="1"/>
+    <col min="2" max="2" width="55.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" customWidth="1"/>
+    <col min="4" max="4" width="20.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.54296875" customWidth="1"/>
+    <col min="6" max="6" width="15.1796875" customWidth="1"/>
+    <col min="7" max="7" width="18.7265625" customWidth="1"/>
+    <col min="8" max="8" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="21">
+    <row r="1" spans="1:7" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="73" t="s">
-        <v>0</v>
+        <v>64</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4333,9 +4333,9 @@
       <c r="E1" s="28"/>
       <c r="F1" s="28"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" s="30"/>
       <c r="C2" s="30"/>
@@ -4343,7 +4343,7 @@
       <c r="E2" s="74"/>
       <c r="F2" s="74"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="29"/>
       <c r="B3" s="31"/>
       <c r="D3" s="92">
@@ -4355,10 +4355,10 @@
         <v>45079</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="19.5" customHeight="1">
+    <row r="4" spans="1:7" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="32"/>
       <c r="B4" s="33" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C4" s="90">
         <v>44812</v>
@@ -4366,26 +4366,26 @@
       <c r="D4" s="90"/>
       <c r="E4" s="75"/>
       <c r="F4" s="32" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G4" s="76">
         <v>45079</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="14.25" customHeight="1">
+    <row r="5" spans="1:7" ht="14.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="32"/>
       <c r="B5" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="91" t="s">
         <v>4</v>
-      </c>
-      <c r="C5" s="91" t="s">
-        <v>5</v>
       </c>
       <c r="D5" s="91"/>
       <c r="E5" s="77"/>
       <c r="F5" s="32"/>
       <c r="G5" s="32"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="34"/>
       <c r="B6" s="34"/>
       <c r="C6" s="34"/>
@@ -4394,35 +4394,35 @@
       <c r="F6" s="34"/>
       <c r="G6" s="34"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="88" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="88" t="s">
+      <c r="C7" s="88" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="88" t="s">
+      <c r="D7" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="88" t="s">
+      <c r="E7" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="88" t="s">
+      <c r="F7" s="88" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="88" t="s">
+      <c r="G7" s="88" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="88" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" s="42">
         <v>1</v>
       </c>
       <c r="B8" s="43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="44"/>
       <c r="D8" s="45">
@@ -4440,16 +4440,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="str">
-        <f t="shared" ref="A9" ca="1" si="2">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A9" si="2">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>14</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>15</v>
       </c>
       <c r="D9" s="4">
         <v>44812</v>
@@ -4466,16 +4466,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.2</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D10" s="4">
         <v>44823</v>
@@ -4492,16 +4492,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.3</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D11" s="4">
         <v>44823</v>
@@ -4518,12 +4518,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="48">
         <v>2</v>
       </c>
       <c r="B12" s="49" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C12" s="50"/>
       <c r="D12" s="51">
@@ -4541,16 +4541,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.1</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C13" s="36" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D13" s="4">
         <v>44827</v>
@@ -4567,16 +4567,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="str">
-        <f t="shared" ref="A14:A19" ca="1" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A14:A19" si="5">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>2.2</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="4">
         <v>44855</v>
@@ -4593,16 +4593,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>2.3</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="4">
         <v>44874</v>
@@ -4619,16 +4619,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>2.4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="9">
         <v>44844</v>
@@ -4645,16 +4645,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:7">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
       <c r="B17" s="35" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="9">
         <v>44844</v>
@@ -4671,16 +4671,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>2.6</v>
       </c>
       <c r="B18" s="35" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="9">
         <v>44855</v>
@@ -4697,16 +4697,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="str">
-        <f t="shared" ca="1" si="5"/>
+        <f t="shared" si="5"/>
         <v>2.7</v>
       </c>
       <c r="B19" s="35" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="9">
         <v>44855</v>
@@ -4723,12 +4723,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="54">
         <v>3</v>
       </c>
       <c r="B20" s="55" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C20" s="56"/>
       <c r="D20" s="57">
@@ -4743,19 +4743,19 @@
       </c>
       <c r="G20" s="59">
         <f t="shared" ca="1" si="6"/>
-        <v>5.1470588235294115E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>0.33088235294117646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="str">
-        <f t="shared" ref="A21:A25" ca="1" si="8">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A21:A25" si="8">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.1</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" s="4">
         <v>44911</v>
@@ -4769,19 +4769,19 @@
       </c>
       <c r="G21" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" si="8"/>
         <v>3.2</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" s="4">
         <v>44911</v>
@@ -4795,19 +4795,19 @@
       </c>
       <c r="G22" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.2.1</v>
       </c>
       <c r="B23" s="38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D23" s="4">
         <v>44918</v>
@@ -4821,19 +4821,19 @@
       </c>
       <c r="G23" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.2.2</v>
       </c>
       <c r="B24" s="38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" s="4">
         <v>44918</v>
@@ -4847,19 +4847,19 @@
       </c>
       <c r="G24" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="str">
-        <f t="shared" ca="1" si="8"/>
+        <f t="shared" si="8"/>
         <v>3.3</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" s="4">
         <v>44911</v>
@@ -4873,19 +4873,19 @@
       </c>
       <c r="G25" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.3.1</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" s="9">
         <v>44911</v>
@@ -4899,19 +4899,19 @@
       </c>
       <c r="G26" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" ht="16.899999999999999" customHeight="1">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="16.899999999999999" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="str">
-        <f t="shared" ref="A27:A32" ca="1" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <f t="shared" ref="A27:A32" si="9">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>3.3.1.1</v>
       </c>
       <c r="B27" s="38" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" s="9">
         <v>44911</v>
@@ -4925,19 +4925,19 @@
       </c>
       <c r="G27" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" si="9"/>
         <v>3.3.1.2</v>
       </c>
       <c r="B28" s="39" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" s="9">
         <v>44911</v>
@@ -4951,19 +4951,19 @@
       </c>
       <c r="G28" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" si="9"/>
         <v>3.3.1.3</v>
       </c>
       <c r="B29" s="39" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D29" s="9">
         <v>44911</v>
@@ -4977,19 +4977,19 @@
       </c>
       <c r="G29" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" si="9"/>
         <v>3.3.1.4</v>
       </c>
       <c r="B30" s="39" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D30" s="9">
         <v>44911</v>
@@ -5003,19 +5003,19 @@
       </c>
       <c r="G30" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" si="9"/>
         <v>3.3.1.5</v>
       </c>
       <c r="B31" s="39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D31" s="9">
         <v>44911</v>
@@ -5029,19 +5029,19 @@
       </c>
       <c r="G31" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="str">
-        <f t="shared" ca="1" si="9"/>
+        <f t="shared" si="9"/>
         <v>3.3.1.6</v>
       </c>
       <c r="B32" s="38" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D32" s="9">
         <v>44911</v>
@@ -5055,19 +5055,19 @@
       </c>
       <c r="G32" s="86">
         <f t="shared" ca="1" si="6"/>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>0.49450549450549453</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.3.2</v>
       </c>
       <c r="B33" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D33" s="9">
         <v>45002</v>
@@ -5084,16 +5084,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>3.4</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D34" s="4">
         <v>45002</v>
@@ -5110,16 +5110,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.4.1</v>
       </c>
       <c r="B35" s="87" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D35" s="4">
         <v>45002</v>
@@ -5136,16 +5136,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>3.4.2</v>
       </c>
       <c r="B36" s="87" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D36" s="4">
         <v>45002</v>
@@ -5162,13 +5162,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="79" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>4</v>
       </c>
       <c r="B37" s="80" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C37" s="81"/>
       <c r="D37" s="82">
@@ -5186,16 +5186,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D38" s="4">
         <v>45047</v>
@@ -5212,16 +5212,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D39" s="4">
         <v>45047</v>
@@ -5238,12 +5238,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" s="60">
         <v>4</v>
       </c>
       <c r="B40" s="61" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C40" s="62"/>
       <c r="D40" s="63">
@@ -5258,19 +5258,19 @@
       </c>
       <c r="G40" s="65">
         <f t="shared" ca="1" si="10"/>
-        <v>0.39700374531835209</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>0.5393258426966292</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="str">
-        <f t="shared" ref="A41" ca="1" si="12">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f t="shared" ref="A41" si="12">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.1</v>
       </c>
       <c r="B41" s="40" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D41" s="4">
         <v>44812</v>
@@ -5287,16 +5287,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.2</v>
       </c>
       <c r="B42" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D42" s="4">
         <v>44827</v>
@@ -5313,16 +5313,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:7">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.2.1</v>
       </c>
       <c r="B43" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D43" s="4">
         <v>44827</v>
@@ -5339,16 +5339,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:7">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.2.2</v>
       </c>
       <c r="B44" s="38" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D44" s="4">
         <v>44827</v>
@@ -5365,16 +5365,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:7">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.2.3</v>
       </c>
       <c r="B45" s="39" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D45" s="4">
         <v>44827</v>
@@ -5391,16 +5391,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:7">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.2.4</v>
       </c>
       <c r="B46" s="37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D46" s="4">
         <v>44827</v>
@@ -5417,16 +5417,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:7">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.3</v>
       </c>
       <c r="B47" s="40" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D47" s="4">
         <v>44844</v>
@@ -5443,16 +5443,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:7">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="str">
-        <f t="shared" ref="A48:A54" ca="1" si="13">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f t="shared" ref="A48:A54" si="13">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>4.3.1</v>
       </c>
       <c r="B48" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D48" s="4">
         <v>44844</v>
@@ -5469,16 +5469,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:7">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" si="13"/>
         <v>4.3.2</v>
       </c>
       <c r="B49" s="66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D49" s="4">
         <v>44844</v>
@@ -5495,16 +5495,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:7">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" si="13"/>
         <v>4.3.3</v>
       </c>
       <c r="B50" s="66" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D50" s="4">
         <v>44844</v>
@@ -5521,16 +5521,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:7">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.4</v>
       </c>
       <c r="B51" s="41" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D51" s="4">
         <v>44876</v>
@@ -5547,16 +5547,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:7">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" si="13"/>
         <v>4.4.1</v>
       </c>
       <c r="B52" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D52" s="4">
         <v>44876</v>
@@ -5573,16 +5573,16 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:7">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.5</v>
       </c>
       <c r="B53" s="41" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D53" s="4">
         <v>44918</v>
@@ -5596,19 +5596,19 @@
       </c>
       <c r="G53" s="86">
         <f t="shared" ca="1" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:7">
+        <v>0.31932773109243695</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="str">
-        <f t="shared" ca="1" si="13"/>
+        <f t="shared" si="13"/>
         <v>4.5.1</v>
       </c>
       <c r="B54" s="38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D54" s="4">
         <v>44918</v>
@@ -5622,19 +5622,19 @@
       </c>
       <c r="G54" s="86">
         <f t="shared" ca="1" si="10"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="1:7">
+        <v>0.31932773109243695</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>4.6</v>
       </c>
       <c r="B55" s="41" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D55" s="4">
         <v>45037</v>
@@ -5651,7 +5651,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" s="1"/>
       <c r="B56" s="14"/>
       <c r="C56" s="14"/>
@@ -5660,7 +5660,7 @@
       <c r="F56" s="15"/>
       <c r="G56" s="16"/>
     </row>
-    <row r="57" spans="1:7">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" s="1"/>
       <c r="B57" s="14"/>
       <c r="C57" s="14"/>
@@ -5669,9 +5669,9 @@
       <c r="F57" s="15"/>
       <c r="G57" s="16"/>
     </row>
-    <row r="58" spans="1:7">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" s="17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B58" s="18"/>
       <c r="C58" s="11"/>
@@ -5680,7 +5680,7 @@
       <c r="F58" s="12"/>
       <c r="G58" s="13"/>
     </row>
-    <row r="59" spans="1:7">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" s="19"/>
       <c r="B59" s="20"/>
       <c r="C59" s="20"/>
@@ -5689,13 +5689,13 @@
       <c r="F59" s="21"/>
       <c r="G59" s="20"/>
     </row>
-    <row r="60" spans="1:7">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" s="22" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),TEXT(VALUE(prevWBS)+1,"#"),TEXT(VALUE(LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1))+1,"#")))</f>
         <v>1</v>
       </c>
       <c r="B60" s="23" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C60" s="24"/>
       <c r="D60" s="4">
@@ -5708,13 +5708,13 @@
       </c>
       <c r="G60" s="6"/>
     </row>
-    <row r="61" spans="1:7">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",1))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",1))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",1))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",2))-FIND("`",SUBSTITUTE(prevWBS,".","`",1))-1)))+1)))</f>
         <v>1.1</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C61" s="26"/>
       <c r="D61" s="4">
@@ -5727,13 +5727,13 @@
       </c>
       <c r="G61" s="6"/>
     </row>
-    <row r="62" spans="1:7">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",2))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",2))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",2))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",3))-FIND("`",SUBSTITUTE(prevWBS,".","`",2))-1)))+1)))</f>
         <v>1.1.1</v>
       </c>
       <c r="B62" s="27" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C62" s="26"/>
       <c r="D62" s="4">
@@ -5746,13 +5746,13 @@
       </c>
       <c r="G62" s="6"/>
     </row>
-    <row r="63" spans="1:7">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="str">
-        <f ca="1">IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
+        <f>IF(ISERROR(VALUE(SUBSTITUTE(prevWBS,".",""))),"0.0.0.1",IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",3))),prevWBS&amp;".1",LEFT(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3)))&amp;IF(ISERROR(FIND("`",SUBSTITUTE(prevWBS,".","`",4))),VALUE(RIGHT(prevWBS,LEN(prevWBS)-FIND("`",SUBSTITUTE(prevWBS,".","`",3))))+1,VALUE(MID(prevWBS,FIND("`",SUBSTITUTE(prevWBS,".","`",3))+1,(FIND("`",SUBSTITUTE(prevWBS,".","`",4))-FIND("`",SUBSTITUTE(prevWBS,".","`",3))-1)))+1)))</f>
         <v>1.1.1.1</v>
       </c>
       <c r="B63" s="27" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C63" s="26"/>
       <c r="D63" s="4">
@@ -5822,6 +5822,17 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2ad1eb1-ab19-48ec-904d-67ddbbca3aa7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="e31cdc8e-fda6-45f3-97f2-c1b384c195ed" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010088CE0F64D6E5D84A8FCDD529D4CCD8E1" ma:contentTypeVersion="11" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="a7e2c6f8e0f1087e219c33faf4b3b507">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="e2ad1eb1-ab19-48ec-904d-67ddbbca3aa7" xmlns:ns3="e31cdc8e-fda6-45f3-97f2-c1b384c195ed" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2b3b37963f88ba6e1017082f35fad5f2" ns2:_="" ns3:_="">
     <xsd:import namespace="e2ad1eb1-ab19-48ec-904d-67ddbbca3aa7"/>
@@ -6032,25 +6043,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e2ad1eb1-ab19-48ec-904d-67ddbbca3aa7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="e31cdc8e-fda6-45f3-97f2-c1b384c195ed" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50431AEA-3F9C-4BE6-93CA-A45E3BCEBE80}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{50431AEA-3F9C-4BE6-93CA-A45E3BCEBE80}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9720485-96E8-4930-BFA2-ED3B4CDE0C14}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2792651-6C39-4551-BF66-5C319D246F8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e2ad1eb1-ab19-48ec-904d-67ddbbca3aa7"/>
+    <ds:schemaRef ds:uri="e31cdc8e-fda6-45f3-97f2-c1b384c195ed"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E2792651-6C39-4551-BF66-5C319D246F8C}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F9720485-96E8-4930-BFA2-ED3B4CDE0C14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="e2ad1eb1-ab19-48ec-904d-67ddbbca3aa7"/>
+    <ds:schemaRef ds:uri="e31cdc8e-fda6-45f3-97f2-c1b384c195ed"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>